<commit_message>
Updated Source Codes 30th Aug 2018
</commit_message>
<xml_diff>
--- a/Presentation/SLV.Web/uploads/Sample/SampleExcelPermissionInBound.xlsx
+++ b/Presentation/SLV.Web/uploads/Sample/SampleExcelPermissionInBound.xlsx
@@ -126,12 +126,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -522,93 +525,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" customWidth="1"/>
-    <col min="5" max="8" width="15" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="2" width="18.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="4" customWidth="1"/>
+    <col min="4" max="6" width="23.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12" style="4" customWidth="1"/>
+    <col min="8" max="12" width="15" style="4" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.140625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" style="4" customWidth="1"/>
+    <col min="20" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="M2" s="2"/>
+      <c r="Q2" s="7"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <hyperlinks>
+    <hyperlink ref="Q7" r:id="rId1" display="https://www.shutterstock.com/pic-154184030/stock-vector-a-vector-illustration-of-happy-kids-helping-their-mother-cleaning-house.html?src=1MtNWbRkaTmCkh_1fZLPrA-2-29"/>
+    <hyperlink ref="Q8" r:id="rId2" display="https://www.shutterstock.com/pic-86604898/stock-vector-halloween-children-trick-or-treating-in-halloween-costume.html?src=tt8dc062voJ9O4I6HCkZ3Q-1-9"/>
+    <hyperlink ref="Q9" r:id="rId3" display="https://www.shutterstock.com/pic-330866894/stock-photo-boy-lying-writing.html?src=xLoqz9DEnXsiE0XV_WVXOg-1-15"/>
+    <hyperlink ref="Q10" r:id="rId4" display="https://www.shutterstock.com/pic-161967581/stock-photo-big-lion-lying-on-savannah-grass-landscape-with-characteristic-trees-on-the-plain-and-hills-in-the-background.html?src=hNqo08ZJ-Vzdo2ydn_UahA-1-7"/>
+    <hyperlink ref="Q11" r:id="rId5" display="https://www.shutterstock.com/pic-453450040/stock-photo-african-elephants-loxodonta-africana-drinking-water-etosha-national-park-namibia.html?src=2G29n6a7JIztXAlcQqlYZA-1-3"/>
+    <hyperlink ref="Q12" r:id="rId6" display="https://www.shutterstock.com/pic-154487144/stock-photo-flamingos-in-the-park-as-xcaret-mexico-latin-america.html?src=8jUFmi4ME8t0zA4u1nRj1w-1-6"/>
+    <hyperlink ref="Q13" r:id="rId7" display="https://www.shutterstock.com/pic-284546228/stock-photo-giraffes-isolated-on-white-background.html?src=aZuNgKoBQ83xlu0NopYPfA-1-30"/>
+    <hyperlink ref="Q14" r:id="rId8" display="http://www.shutterstock.com/pic.mhtml?id=141311467&amp;src=id"/>
+    <hyperlink ref="Q16" r:id="rId9" display="http://www.gettyimages.in/license/89859534"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>